<commit_message>
Simplified methods by adding getXbyId to CyclingPortal, updated cover page spreadsheet
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dojoe\Documents\Uni\(ECM1410) Object-Oriented Programming\Course Work\new_ecm1410_coursework\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM1410/ecm1410_coursework/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9B362039-1F43-491E-8103-9F94DD47F917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{9B362039-1F43-491E-8103-9F94DD47F917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F50066D-5665-4898-9AA9-0FCA5B78FFC3}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,14 +35,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
   <si>
-    <t>Stuent ID</t>
-  </si>
-  <si>
     <t>Weight</t>
   </si>
   <si>
@@ -59,6 +56,12 @@
   </si>
   <si>
     <t>OO Design</t>
+  </si>
+  <si>
+    <t>OO Design + Implementation</t>
+  </si>
+  <si>
+    <t>Student ID</t>
   </si>
 </sst>
 </file>
@@ -141,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -155,25 +158,28 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -493,37 +499,40 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.21875" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C3" s="8" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C3" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="8"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="E5" s="4">
         <v>710022765</v>
@@ -533,10 +542,10 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E6" s="5">
         <v>0.5</v>
@@ -546,31 +555,31 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C8" s="7" t="s">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C8" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>6</v>
       </c>
       <c r="F9" s="1">
         <v>710022765</v>
@@ -579,80 +588,90 @@
         <v>710033804</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C10" s="9">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C10" s="7">
         <v>44616</v>
       </c>
-      <c r="D10" s="10">
+      <c r="D10" s="8">
         <v>0.52083333333333337</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>1.25</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C11" s="7">
+        <v>44622</v>
+      </c>
+      <c r="D11" s="14">
+        <v>0.4375</v>
+      </c>
+      <c r="E11" s="9">
+        <v>2</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="G10" s="11" t="s">
+      <c r="G11" s="9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="11"/>
-      <c r="D11" s="13"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="11"/>
-    </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C12" s="11"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="11"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="11"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="11"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C14" s="11"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="11"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="11"/>
-    </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="11"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="11"/>
-    </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="11"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="11"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="11"/>
-    </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" s="11"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="11"/>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C12" s="9"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="9"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="9"/>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="9"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="9"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C14" s="9"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="9"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="9"/>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C15" s="9"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="9"/>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C16" s="9"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="9"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="9"/>
+    </row>
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+      <c r="C17" s="9"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="9"/>
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>

<commit_message>
Added to the cover page
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM1410/ecm1410_coursework/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dojoe\Documents\Uni\(ECM1410) Object-Oriented Programming\Course Work\ecm1410_coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="29" documentId="8_{9B362039-1F43-491E-8103-9F94DD47F917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6F50066D-5665-4898-9AA9-0FCA5B78FFC3}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -173,13 +173,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -499,37 +499,37 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.21875" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C3" s="13" t="s">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -542,7 +542,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
@@ -555,23 +555,23 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C8" s="12" t="s">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="12"/>
-    </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="D8" s="13"/>
+      <c r="E8" s="13"/>
+      <c r="F8" s="13"/>
+      <c r="G8" s="13"/>
+    </row>
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +588,7 @@
         <v>710033804</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
         <v>44616</v>
       </c>
@@ -605,11 +605,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="7">
         <v>44622</v>
       </c>
-      <c r="D11" s="14">
+      <c r="D11" s="12">
         <v>0.4375</v>
       </c>
       <c r="E11" s="9">
@@ -622,56 +622,66 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C12" s="9"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="7">
+        <v>44630</v>
+      </c>
+      <c r="D12" s="12">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E12" s="9">
+        <v>1.25</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="9"/>
       <c r="D13" s="11"/>
       <c r="E13" s="9"/>
       <c r="F13" s="11"/>
       <c r="G13" s="9"/>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="9"/>
       <c r="F14" s="11"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
       <c r="F15" s="11"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="11"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
       <c r="F17" s="11"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>

<commit_message>
Added more methods to CyclingPortal
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dojoe\Documents\Uni\(ECM1410) Object-Oriented Programming\Course Work\ecm1410_coursework\res\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM1410/ecm1410_coursework/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F204240E-E05D-45D3-8104-482049B5C27E}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -144,7 +144,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
@@ -182,6 +182,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,20 +500,20 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="16.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="25.28515625" customWidth="1"/>
-    <col min="6" max="6" width="28.28515625" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" customWidth="1"/>
-    <col min="8" max="8" width="8.85546875" customWidth="1"/>
+    <col min="5" max="5" width="25.33203125" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" customWidth="1"/>
+    <col min="8" max="8" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
@@ -522,14 +523,14 @@
       <c r="G3" s="14"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -542,7 +543,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
@@ -555,14 +556,14 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C8" s="13" t="s">
         <v>2</v>
       </c>
@@ -571,7 +572,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -588,7 +589,7 @@
         <v>710033804</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C10" s="7">
         <v>44616</v>
       </c>
@@ -605,7 +606,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C11" s="7">
         <v>44622</v>
       </c>
@@ -622,7 +623,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C12" s="7">
         <v>44630</v>
       </c>
@@ -639,49 +640,59 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C13" s="9"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="9"/>
-    </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+      <c r="C13" s="7">
+        <v>44631</v>
+      </c>
+      <c r="D13" s="15">
+        <v>0.4375</v>
+      </c>
+      <c r="E13" s="9">
+        <v>1</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C14" s="9"/>
       <c r="D14" s="11"/>
       <c r="E14" s="9"/>
       <c r="F14" s="11"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
       <c r="F15" s="11"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C16" s="9"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="11"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C17" s="9"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
       <c r="F17" s="11"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>

<commit_message>
Added to cover page
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM1410/ecm1410_coursework/res/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dojoe\Documents\Uni\(ECM1410) Object-Oriented Programming\Course Work\ecm1410_coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F204240E-E05D-45D3-8104-482049B5C27E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DCDF60-0749-43C8-AD8C-E9ECD674BB4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -182,7 +182,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,20 +502,20 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="16.5546875" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" customWidth="1"/>
-    <col min="6" max="6" width="28.33203125" customWidth="1"/>
-    <col min="7" max="7" width="27.5546875" customWidth="1"/>
-    <col min="8" max="8" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" customWidth="1"/>
+    <col min="6" max="6" width="28.28515625" customWidth="1"/>
+    <col min="7" max="7" width="27.5703125" customWidth="1"/>
+    <col min="8" max="8" width="8.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C3" s="14" t="s">
         <v>0</v>
       </c>
@@ -523,14 +525,14 @@
       <c r="G3" s="14"/>
       <c r="H3" s="3"/>
     </row>
-    <row r="4" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
     </row>
-    <row r="5" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="2"/>
       <c r="D5" s="6" t="s">
         <v>8</v>
@@ -543,7 +545,7 @@
       </c>
       <c r="G5" s="2"/>
     </row>
-    <row r="6" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C6" s="2"/>
       <c r="D6" s="6" t="s">
         <v>1</v>
@@ -556,14 +558,14 @@
       </c>
       <c r="G6" s="2"/>
     </row>
-    <row r="7" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
     </row>
-    <row r="8" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C8" s="13" t="s">
         <v>2</v>
       </c>
@@ -572,7 +574,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
     </row>
-    <row r="9" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C9" s="1" t="s">
         <v>3</v>
       </c>
@@ -589,7 +591,7 @@
         <v>710033804</v>
       </c>
     </row>
-    <row r="10" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="7">
         <v>44616</v>
       </c>
@@ -606,7 +608,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C11" s="7">
         <v>44622</v>
       </c>
@@ -623,7 +625,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C12" s="7">
         <v>44630</v>
       </c>
@@ -640,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C13" s="7">
         <v>44631</v>
       </c>
@@ -657,42 +659,46 @@
         <v>7</v>
       </c>
     </row>
-    <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="7">
+        <v>44636</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.4375</v>
+      </c>
       <c r="E14" s="9"/>
       <c r="F14" s="11"/>
       <c r="G14" s="9"/>
     </row>
-    <row r="15" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C15" s="9"/>
       <c r="D15" s="11"/>
       <c r="E15" s="9"/>
       <c r="F15" s="11"/>
       <c r="G15" s="9"/>
     </row>
-    <row r="16" spans="3:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>
       <c r="D16" s="11"/>
       <c r="E16" s="9"/>
       <c r="F16" s="11"/>
       <c r="G16" s="9"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C17" s="9"/>
       <c r="D17" s="11"/>
       <c r="E17" s="9"/>
       <c r="F17" s="11"/>
       <c r="G17" s="9"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
       <c r="G18" s="2"/>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>

</xml_diff>

<commit_message>
Implemented more methods in CyclingPortal
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/ac1198_exeter_ac_uk/Documents/Documents/ECM1410/ecm1410_coursework/res/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F204240E-E05D-45D3-8104-482049B5C27E}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="13_ncr:1_{0C864907-69E8-40F3-ADA4-DF197DF3BEFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E3C65485-0934-4645-9D24-481A06F0C9B3}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>Student ID</t>
+  </si>
+  <si>
+    <t>Implementation</t>
   </si>
 </sst>
 </file>
@@ -182,7 +185,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -658,11 +663,21 @@
       </c>
     </row>
     <row r="14" spans="3:8" x14ac:dyDescent="0.3">
-      <c r="C14" s="9"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="9"/>
-      <c r="F14" s="11"/>
-      <c r="G14" s="9"/>
+      <c r="C14" s="7">
+        <v>44636</v>
+      </c>
+      <c r="D14" s="12">
+        <v>0.4375</v>
+      </c>
+      <c r="E14" s="9">
+        <v>3</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.3">
       <c r="C15" s="9"/>

</xml_diff>

<commit_message>
Added functionality & cover sheet
</commit_message>
<xml_diff>
--- a/res/ecm1410_cover_page.xlsx
+++ b/res/ecm1410_cover_page.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dojoe\Documents\Uni\(ECM1410) Object-Oriented Programming\Course Work\ecm1410_coursework\res\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7509ACC6-F566-4586-81EE-57CDDC9F0AA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C1EBB-AD4F-4055-8AE3-2BFA1143977B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{433A8149-F100-4901-A21D-4D03AA21A4E8}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="10">
   <si>
     <t>ECM1410 Cover Page</t>
   </si>
@@ -505,7 +505,7 @@
   <dimension ref="C3:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,11 +680,21 @@
       </c>
     </row>
     <row r="15" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="9"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="9"/>
+      <c r="C15" s="7">
+        <v>44637</v>
+      </c>
+      <c r="D15" s="12">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="16" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C16" s="9"/>

</xml_diff>